<commit_message>
Uprava vyplnovaciho listku pro pololetni test
</commit_message>
<xml_diff>
--- a/testy/vyplnovaci_listek.xlsx
+++ b/testy/vyplnovaci_listek.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="zaverecny" sheetId="1" r:id="rId1"/>
+    <sheet name="pololeti" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Jméno:</t>
   </si>
@@ -36,6 +37,12 @@
   </si>
   <si>
     <t>Testová část</t>
+  </si>
+  <si>
+    <t>Testová část - 0,5 b / odpověď</t>
+  </si>
+  <si>
+    <t>Písemná část - 1,5 b / odpověď</t>
   </si>
 </sst>
 </file>
@@ -163,9 +170,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -176,6 +180,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,14 +466,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="5" customWidth="1"/>
-    <col min="2" max="9" width="9.140625" style="9"/>
+    <col min="2" max="9" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -486,19 +493,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
@@ -511,7 +518,7 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
@@ -524,7 +531,7 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5" s="3"/>
@@ -537,7 +544,7 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
@@ -550,7 +557,7 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
@@ -563,7 +570,7 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="3"/>
@@ -576,7 +583,7 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9" s="3"/>
@@ -589,7 +596,7 @@
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
       <c r="B10" s="3"/>
@@ -602,7 +609,7 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
       <c r="B11" s="3"/>
@@ -616,88 +623,88 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>1</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>5</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <v>9</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>2</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>6</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="11">
+      <c r="G14" s="10">
         <v>10</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>3</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>7</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <v>11</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>4</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>8</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <v>12</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="7"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
@@ -707,7 +714,7 @@
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>13</v>
       </c>
       <c r="B18" s="3"/>
@@ -720,7 +727,7 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>14</v>
       </c>
       <c r="B19" s="3"/>
@@ -733,7 +740,7 @@
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>15</v>
       </c>
       <c r="B20" s="3"/>
@@ -746,7 +753,7 @@
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>16</v>
       </c>
       <c r="B21" s="3"/>
@@ -759,7 +766,7 @@
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>17</v>
       </c>
       <c r="B22" s="3"/>
@@ -772,7 +779,7 @@
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>18</v>
       </c>
       <c r="B23" s="3"/>
@@ -785,7 +792,7 @@
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>19</v>
       </c>
       <c r="B24" s="3"/>
@@ -798,7 +805,7 @@
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>20</v>
       </c>
       <c r="B25" s="3"/>
@@ -811,7 +818,7 @@
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>21</v>
       </c>
       <c r="B26" s="3"/>
@@ -831,4 +838,181 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="5" customWidth="1"/>
+    <col min="2" max="9" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="10">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="10">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="10">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B9:I9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testy: - vyplnovaci listky
</commit_message>
<xml_diff>
--- a/testy/vyplnovaci_listek.xlsx
+++ b/testy/vyplnovaci_listek.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="zaverecny" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Jméno:</t>
   </si>
@@ -33,16 +33,19 @@
     <t>Varianta:</t>
   </si>
   <si>
-    <t>Písemná část</t>
-  </si>
-  <si>
-    <t>Testová část</t>
-  </si>
-  <si>
     <t>Testová část - 0,5 b / odpověď</t>
   </si>
   <si>
     <t>Písemná část - 1,5 b / odpověď</t>
+  </si>
+  <si>
+    <t>Písemná část - 1,5 b</t>
+  </si>
+  <si>
+    <t>Testová část - 0,5 b</t>
+  </si>
+  <si>
+    <t>Testová část - 1 b</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -154,11 +157,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -182,6 +218,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,16 +544,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="B2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
@@ -623,16 +674,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="B12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
@@ -641,12 +692,12 @@
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
       <c r="D13" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
       <c r="G13" s="10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="4"/>
@@ -658,12 +709,12 @@
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
       <c r="D14" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
       <c r="G14" s="10">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="4"/>
@@ -675,12 +726,12 @@
       <c r="B15" s="2"/>
       <c r="C15" s="4"/>
       <c r="D15" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
       <c r="G15" s="10">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="4"/>
@@ -692,56 +743,60 @@
       <c r="B16" s="2"/>
       <c r="C16" s="4"/>
       <c r="D16" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="10">
-        <v>12</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="4"/>
+      <c r="G16" s="17">
+        <v>14</v>
+      </c>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="7"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>13</v>
-      </c>
-      <c r="B18" s="3"/>
+      <c r="A17" s="9">
+        <v>5</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17">
+        <v>10</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>14</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="12"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -752,9 +807,9 @@
       <c r="H20" s="3"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -765,9 +820,9 @@
       <c r="H21" s="3"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -778,9 +833,9 @@
       <c r="H22" s="3"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -791,9 +846,9 @@
       <c r="H23" s="3"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -804,9 +859,9 @@
       <c r="H24" s="3"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -817,9 +872,9 @@
       <c r="H25" s="3"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -830,10 +885,37 @@
       <c r="H26" s="3"/>
       <c r="I26" s="4"/>
     </row>
+    <row r="27" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>23</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -844,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -871,16 +953,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="B2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
@@ -962,16 +1044,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="B9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9">

</xml_diff>